<commit_message>
Finish accounting for custom
</commit_message>
<xml_diff>
--- a/document/FORM BANG KE  NHA THAU.xlsx
+++ b/document/FORM BANG KE  NHA THAU.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Working\Projects\GitHub\ael\document\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="75" windowWidth="9495" windowHeight="6915"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>BẢNG KÊ VẬN CHUYỂN</t>
   </si>
@@ -80,6 +85,9 @@
   </si>
   <si>
     <t>Thành tiền</t>
+  </si>
+  <si>
+    <t>Flexible?</t>
   </si>
 </sst>
 </file>
@@ -149,7 +157,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -162,8 +170,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -186,6 +200,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -234,7 +257,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -256,9 +279,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -272,6 +292,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -328,6 +354,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -375,7 +404,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -410,7 +439,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -622,7 +651,7 @@
   <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,24 +664,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
@@ -691,10 +720,12 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
+      <c r="M3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
@@ -730,31 +761,31 @@
       <c r="J4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="K4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="M4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="N4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="11" t="s">
+      <c r="O4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="P4" s="11" t="s">
+      <c r="P4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="12" t="s">
+      <c r="Q4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="R4" s="12" t="s">
+      <c r="R4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="S4" s="13" t="s">
+      <c r="S4" s="12" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1173,8 +1204,9 @@
       <c r="S22" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:P1"/>
+    <mergeCell ref="M3:P3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
add new report templates
</commit_message>
<xml_diff>
--- a/document/FORM BANG KE  NHA THAU.xlsx
+++ b/document/FORM BANG KE  NHA THAU.xlsx
@@ -291,17 +291,17 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -653,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,27 +667,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
     </row>
     <row r="2" spans="1:19" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
@@ -723,12 +723,12 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="14" t="s">
+      <c r="M3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
@@ -770,7 +770,7 @@
       <c r="L4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="16" t="s">
+      <c r="M4" s="14" t="s">
         <v>10</v>
       </c>
       <c r="N4" s="9" t="s">
@@ -782,10 +782,10 @@
       <c r="P4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="15" t="s">
+      <c r="Q4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="R4" s="15" t="s">
+      <c r="R4" s="13" t="s">
         <v>17</v>
       </c>
       <c r="S4" s="11" t="s">
@@ -1208,8 +1208,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:P1"/>
     <mergeCell ref="M3:P3"/>
+    <mergeCell ref="A1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>